<commit_message>
fixed undefined object bug
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Round 1/Beginner.xlsx
+++ b/public/res/leaderboards/Round 1/Beginner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamzaqureshi/Documents/Programming/Python/poker-tournament-leaderboard/public/res/leaderboards/Round 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B406E2-0AA2-8540-A56C-D653F8442818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABC0A83-2987-244F-A38B-166EF091C2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>#</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Sicong Chen</t>
   </si>
   <si>
-    <t>Smith (Pagnarasmey) Pit</t>
-  </si>
-  <si>
     <t>Soon Wei Tan</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Benson</t>
+  </si>
+  <si>
+    <t>Smith Pit</t>
   </si>
 </sst>
 </file>
@@ -173,6 +173,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -517,13 +518,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -574,7 +580,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -607,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -618,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -629,7 +635,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -640,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -651,7 +657,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -662,7 +668,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -673,7 +679,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -684,7 +690,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -695,7 +701,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -706,7 +712,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -717,7 +723,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -728,7 +734,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -739,7 +745,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -750,7 +756,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -761,7 +767,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -772,7 +778,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -783,7 +789,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -794,7 +800,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -805,7 +811,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -816,7 +822,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -827,7 +833,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -838,7 +844,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -849,7 +855,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -860,7 +866,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -871,7 +877,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -882,7 +888,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -893,7 +899,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -904,7 +910,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -915,7 +921,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -992,31 +998,9 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45">
         <v>0</v>
       </c>
     </row>

</xml_diff>